<commit_message>
Unified range selection on all commands that operate on ranges using Resolve-XLRange Untested and could use some cleanup/improvements.
</commit_message>
<xml_diff>
--- a/test/data/WithNamedRange.xlsx
+++ b/test/data/WithNamedRange.xlsx
@@ -9,13 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10550"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10550" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="FileScope">Sheet2!$B$2</definedName>
     <definedName name="Name">Sheet1!$B$2:$D$4</definedName>
+    <definedName name="Sheet1Scope" localSheetId="0">Sheet2!$B$3</definedName>
+    <definedName name="Sheet2Scope" localSheetId="1">Sheet2!$B$4</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,6 +28,20 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>File</t>
+  </si>
+  <si>
+    <t>Sheet1</t>
+  </si>
+  <si>
+    <t>Sheet2</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -375,12 +393,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>